<commit_message>
label thermocouple I/O pins
</commit_message>
<xml_diff>
--- a/Hardware/stripboard-PID-Arduino-shield-layout.xlsx
+++ b/Hardware/stripboard-PID-Arduino-shield-layout.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="49">
   <si>
     <t>Top view</t>
   </si>
@@ -538,8 +538,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="451">
+  <cellStyleXfs count="465">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1283,7 +1297,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="451">
+  <cellStyles count="465">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1509,6 +1523,13 @@
     <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="462" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1734,6 +1755,13 @@
     <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="455" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="457" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="459" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="461" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2848,128 +2876,128 @@
       </c>
       <c r="B26" s="98"/>
       <c r="C26" s="72" t="str">
-        <f>IF(C$19="X","X","==")</f>
+        <f t="shared" ref="C26:AF26" si="0">IF(C$19="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="D26" s="73" t="str">
-        <f>IF(D$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="E26" s="73" t="str">
-        <f>IF(E$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="F26" s="73" t="str">
-        <f>IF(F$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="G26" s="73" t="str">
-        <f>IF(G$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="H26" s="73" t="str">
-        <f>IF(H$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="I26" s="73" t="str">
-        <f>IF(I$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="J26" s="73" t="str">
-        <f>IF(J$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="K26" s="73" t="str">
-        <f>IF(K$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="L26" s="73" t="str">
-        <f>IF(L$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="M26" s="73" t="str">
-        <f>IF(M$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="N26" s="73" t="str">
-        <f>IF(N$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="O26" s="73" t="str">
-        <f>IF(O$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="P26" s="73" t="str">
-        <f>IF(P$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="Q26" s="73" t="str">
-        <f>IF(Q$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="R26" s="73" t="str">
-        <f>IF(R$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="S26" s="73" t="str">
-        <f>IF(S$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="T26" s="73" t="str">
-        <f>IF(T$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="U26" s="73" t="str">
-        <f>IF(U$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="V26" s="73" t="str">
-        <f>IF(V$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="W26" s="73" t="str">
-        <f>IF(W$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="X26" s="73" t="str">
-        <f>IF(X$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="Y26" s="73" t="str">
-        <f>IF(Y$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="Z26" s="73" t="str">
-        <f>IF(Z$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AA26" s="73" t="str">
-        <f>IF(AA$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AB26" s="73" t="str">
-        <f>IF(AB$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AC26" s="73" t="str">
-        <f>IF(AC$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AD26" s="73" t="str">
-        <f>IF(AD$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AE26" s="73" t="str">
-        <f>IF(AE$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AF26" s="74" t="str">
-        <f>IF(AF$19="X","X","==")</f>
+        <f t="shared" si="0"/>
         <v>==</v>
       </c>
       <c r="AG26" s="98"/>
       <c r="AH26" s="109" t="str">
-        <f t="shared" ref="AH26" si="0">CONCATENATE(AH$19)</f>
+        <f t="shared" ref="AH26" si="1">CONCATENATE(AH$19)</f>
         <v>AH19</v>
       </c>
     </row>
@@ -2979,2205 +3007,2205 @@
         <v/>
       </c>
       <c r="B27" s="101" t="str">
-        <f t="shared" ref="B27:AH27" si="1">CONCATENATE(B$18)</f>
+        <f t="shared" ref="B27:AH27" si="2">CONCATENATE(B$18)</f>
         <v/>
       </c>
       <c r="C27" s="75" t="str">
-        <f>IF(C$18="X","X","==")</f>
+        <f t="shared" ref="C27:AF27" si="3">IF(C$18="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="D27" s="77" t="str">
-        <f>IF(D$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="E27" s="77" t="str">
-        <f>IF(E$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="F27" s="77" t="str">
-        <f>IF(F$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="G27" s="77" t="str">
-        <f>IF(G$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="H27" s="77" t="str">
-        <f>IF(H$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="I27" s="77" t="str">
-        <f>IF(I$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="J27" s="77" t="str">
-        <f>IF(J$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="K27" s="77" t="str">
-        <f>IF(K$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="L27" s="77" t="str">
-        <f>IF(L$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="M27" s="77" t="str">
-        <f>IF(M$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="N27" s="78" t="str">
-        <f>IF(N$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>X</v>
       </c>
       <c r="O27" s="77" t="str">
-        <f>IF(O$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="P27" s="77" t="str">
-        <f>IF(P$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="Q27" s="77" t="str">
-        <f>IF(Q$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="R27" s="77" t="str">
-        <f>IF(R$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="S27" s="77" t="str">
-        <f>IF(S$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="T27" s="77" t="str">
-        <f>IF(T$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="U27" s="77" t="str">
-        <f>IF(U$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="V27" s="77" t="str">
-        <f>IF(V$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="W27" s="77" t="str">
-        <f>IF(W$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="X27" s="77" t="str">
-        <f>IF(X$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="Y27" s="77" t="str">
-        <f>IF(Y$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="Z27" s="77" t="str">
-        <f>IF(Z$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AA27" s="77" t="str">
-        <f>IF(AA$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AB27" s="77" t="str">
-        <f>IF(AB$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AC27" s="77" t="str">
-        <f>IF(AC$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AD27" s="77" t="str">
-        <f>IF(AD$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AE27" s="77" t="str">
-        <f>IF(AE$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AF27" s="76" t="str">
-        <f>IF(AF$18="X","X","==")</f>
+        <f t="shared" si="3"/>
         <v>==</v>
       </c>
       <c r="AG27" s="101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="AH27" s="104" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:34" s="2" customFormat="1">
       <c r="A28" s="24" t="str">
-        <f>IF(A$17="X","X","==")</f>
+        <f t="shared" ref="A28:AH28" si="4">IF(A$17="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B28" s="25" t="str">
-        <f>IF(B$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="C28" s="77" t="str">
-        <f>IF(C$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="D28" s="77" t="str">
-        <f>IF(D$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="E28" s="77" t="str">
-        <f>IF(E$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="F28" s="77" t="str">
-        <f>IF(F$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="G28" s="77" t="str">
-        <f>IF(G$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="H28" s="78" t="str">
-        <f>IF(H$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>X</v>
       </c>
       <c r="I28" s="77" t="str">
-        <f>IF(I$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="J28" s="77" t="str">
-        <f>IF(J$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="K28" s="77" t="str">
-        <f>IF(K$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="L28" s="77" t="str">
-        <f>IF(L$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="M28" s="77" t="str">
-        <f>IF(M$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="N28" s="77" t="str">
-        <f>IF(N$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="O28" s="77" t="str">
-        <f>IF(O$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="P28" s="77" t="str">
-        <f>IF(P$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="Q28" s="77" t="str">
-        <f>IF(Q$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="R28" s="77" t="str">
-        <f>IF(R$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="S28" s="77" t="str">
-        <f>IF(S$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="T28" s="77" t="str">
-        <f>IF(T$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="U28" s="77" t="str">
-        <f>IF(U$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="V28" s="77" t="str">
-        <f>IF(V$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="W28" s="77" t="str">
-        <f>IF(W$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="X28" s="77" t="str">
-        <f>IF(X$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="Y28" s="77" t="str">
-        <f>IF(Y$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="Z28" s="77" t="str">
-        <f>IF(Z$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AA28" s="77" t="str">
-        <f>IF(AA$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AB28" s="77" t="str">
-        <f>IF(AB$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AC28" s="77" t="str">
-        <f>IF(AC$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AD28" s="77" t="str">
-        <f>IF(AD$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AE28" s="77" t="str">
-        <f>IF(AE$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AF28" s="77" t="str">
-        <f>IF(AF$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AG28" s="25" t="str">
-        <f>IF(AG$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
       <c r="AH28" s="26" t="str">
-        <f>IF(AH$17="X","X","==")</f>
+        <f t="shared" si="4"/>
         <v>==</v>
       </c>
     </row>
     <row r="29" spans="1:34" s="2" customFormat="1">
       <c r="A29" s="27" t="str">
-        <f>IF(A$16="X","X","==")</f>
+        <f t="shared" ref="A29:AH29" si="5">IF(A$16="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B29" s="32" t="str">
-        <f>IF(B$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="C29" s="77" t="str">
-        <f>IF(C$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="D29" s="77" t="str">
-        <f>IF(D$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="E29" s="77" t="str">
-        <f>IF(E$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="F29" s="78" t="str">
-        <f>IF(F$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>X</v>
       </c>
       <c r="G29" s="77" t="str">
-        <f>IF(G$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="H29" s="77" t="str">
-        <f>IF(H$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="I29" s="77" t="str">
-        <f>IF(I$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="J29" s="77" t="str">
-        <f>IF(J$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="K29" s="77" t="str">
-        <f>IF(K$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="L29" s="77" t="str">
-        <f>IF(L$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="M29" s="77" t="str">
-        <f>IF(M$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="N29" s="78" t="str">
-        <f>IF(N$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>X</v>
       </c>
       <c r="O29" s="77" t="str">
-        <f>IF(O$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="P29" s="77" t="str">
-        <f>IF(P$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="Q29" s="77" t="str">
-        <f>IF(Q$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="R29" s="77" t="str">
-        <f>IF(R$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="S29" s="77" t="str">
-        <f>IF(S$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="T29" s="77" t="str">
-        <f>IF(T$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="U29" s="77" t="str">
-        <f>IF(U$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="V29" s="77" t="str">
-        <f>IF(V$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="W29" s="77" t="str">
-        <f>IF(W$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="X29" s="77" t="str">
-        <f>IF(X$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="Y29" s="77" t="str">
-        <f>IF(Y$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="Z29" s="77" t="str">
-        <f>IF(Z$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AA29" s="77" t="str">
-        <f>IF(AA$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AB29" s="77" t="str">
-        <f>IF(AB$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AC29" s="77" t="str">
-        <f>IF(AC$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AD29" s="77" t="str">
-        <f>IF(AD$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AE29" s="77" t="str">
-        <f>IF(AE$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AF29" s="77" t="str">
-        <f>IF(AF$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AG29" s="32" t="str">
-        <f>IF(AG$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
       <c r="AH29" s="28" t="str">
-        <f>IF(AH$16="X","X","==")</f>
+        <f t="shared" si="5"/>
         <v>==</v>
       </c>
     </row>
     <row r="30" spans="1:34" s="2" customFormat="1">
       <c r="A30" s="27" t="str">
-        <f>IF(A$15="X","X","==")</f>
+        <f t="shared" ref="A30:AH30" si="6">IF(A$15="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B30" s="32" t="str">
-        <f>IF(B$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="C30" s="77" t="str">
-        <f>IF(C$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="D30" s="77" t="str">
-        <f>IF(D$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="E30" s="77" t="str">
-        <f>IF(E$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="F30" s="77" t="str">
-        <f>IF(F$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="G30" s="77" t="str">
-        <f>IF(G$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="H30" s="77" t="str">
-        <f>IF(H$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="I30" s="77" t="str">
-        <f>IF(I$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="J30" s="77" t="str">
-        <f>IF(J$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="K30" s="77" t="str">
-        <f>IF(K$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="L30" s="77" t="str">
-        <f>IF(L$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="M30" s="77" t="str">
-        <f>IF(M$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="N30" s="77" t="str">
-        <f>IF(N$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="O30" s="77" t="str">
-        <f>IF(O$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="P30" s="77" t="str">
-        <f>IF(P$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="Q30" s="77" t="str">
-        <f>IF(Q$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="R30" s="77" t="str">
-        <f>IF(R$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="S30" s="77" t="str">
-        <f>IF(S$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="T30" s="77" t="str">
-        <f>IF(T$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="U30" s="77" t="str">
-        <f>IF(U$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="V30" s="77" t="str">
-        <f>IF(V$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="W30" s="77" t="str">
-        <f>IF(W$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="X30" s="77" t="str">
-        <f>IF(X$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="Y30" s="77" t="str">
-        <f>IF(Y$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="Z30" s="77" t="str">
-        <f>IF(Z$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AA30" s="77" t="str">
-        <f>IF(AA$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AB30" s="77" t="str">
-        <f>IF(AB$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AC30" s="77" t="str">
-        <f>IF(AC$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AD30" s="77" t="str">
-        <f>IF(AD$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AE30" s="77" t="str">
-        <f>IF(AE$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AF30" s="77" t="str">
-        <f>IF(AF$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AG30" s="32" t="str">
-        <f>IF(AG$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
       <c r="AH30" s="28" t="str">
-        <f>IF(AH$15="X","X","==")</f>
+        <f t="shared" si="6"/>
         <v>==</v>
       </c>
     </row>
     <row r="31" spans="1:34" s="2" customFormat="1">
       <c r="A31" s="27" t="str">
-        <f>IF(A$14="X","X","==")</f>
+        <f t="shared" ref="A31:AH31" si="7">IF(A$14="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B31" s="32" t="str">
-        <f>IF(B$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="C31" s="77" t="str">
-        <f>IF(C$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="D31" s="77" t="str">
-        <f>IF(D$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="E31" s="77" t="str">
-        <f>IF(E$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="F31" s="77" t="str">
-        <f>IF(F$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="G31" s="77" t="str">
-        <f>IF(G$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="H31" s="77" t="str">
-        <f>IF(H$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="I31" s="77" t="str">
-        <f>IF(I$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="J31" s="77" t="str">
-        <f>IF(J$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="K31" s="77" t="str">
-        <f>IF(K$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="L31" s="77" t="str">
-        <f>IF(L$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="M31" s="77" t="str">
-        <f>IF(M$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="N31" s="78" t="str">
-        <f>IF(N$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>X</v>
       </c>
       <c r="O31" s="77" t="str">
-        <f>IF(O$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="P31" s="77" t="str">
-        <f>IF(P$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="Q31" s="77" t="str">
-        <f>IF(Q$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="R31" s="77" t="str">
-        <f>IF(R$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="S31" s="77" t="str">
-        <f>IF(S$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="T31" s="77" t="str">
-        <f>IF(T$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="U31" s="77" t="str">
-        <f>IF(U$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="V31" s="77" t="str">
-        <f>IF(V$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="W31" s="77" t="str">
-        <f>IF(W$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="X31" s="77" t="str">
-        <f>IF(X$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="Y31" s="77" t="str">
-        <f>IF(Y$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="Z31" s="77" t="str">
-        <f>IF(Z$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AA31" s="77" t="str">
-        <f>IF(AA$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AB31" s="77" t="str">
-        <f>IF(AB$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AC31" s="77" t="str">
-        <f>IF(AC$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AD31" s="77" t="str">
-        <f>IF(AD$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AE31" s="77" t="str">
-        <f>IF(AE$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AF31" s="77" t="str">
-        <f>IF(AF$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AG31" s="32" t="str">
-        <f>IF(AG$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
       <c r="AH31" s="28" t="str">
-        <f>IF(AH$14="X","X","==")</f>
+        <f t="shared" si="7"/>
         <v>==</v>
       </c>
     </row>
     <row r="32" spans="1:34" s="2" customFormat="1">
       <c r="A32" s="27" t="str">
-        <f>IF(A$13="X","X","==")</f>
+        <f t="shared" ref="A32:AH32" si="8">IF(A$13="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B32" s="32" t="str">
-        <f>IF(B$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="C32" s="77" t="str">
-        <f>IF(C$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="D32" s="77" t="str">
-        <f>IF(D$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="E32" s="77" t="str">
-        <f>IF(E$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="F32" s="77" t="str">
-        <f>IF(F$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="G32" s="77" t="str">
-        <f>IF(G$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="H32" s="77" t="str">
-        <f>IF(H$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="I32" s="77" t="str">
-        <f>IF(I$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="J32" s="77" t="str">
-        <f>IF(J$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="K32" s="77" t="str">
-        <f>IF(K$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="L32" s="77" t="str">
-        <f>IF(L$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="M32" s="77" t="str">
-        <f>IF(M$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="N32" s="78" t="str">
-        <f>IF(N$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>X</v>
       </c>
       <c r="O32" s="77" t="str">
-        <f>IF(O$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="P32" s="77" t="str">
-        <f>IF(P$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="Q32" s="77" t="str">
-        <f>IF(Q$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="R32" s="77" t="str">
-        <f>IF(R$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="S32" s="77" t="str">
-        <f>IF(S$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="T32" s="77" t="str">
-        <f>IF(T$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="U32" s="77" t="str">
-        <f>IF(U$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="V32" s="77" t="str">
-        <f>IF(V$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="W32" s="77" t="str">
-        <f>IF(W$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="X32" s="77" t="str">
-        <f>IF(X$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="Y32" s="77" t="str">
-        <f>IF(Y$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="Z32" s="77" t="str">
-        <f>IF(Z$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AA32" s="77" t="str">
-        <f>IF(AA$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AB32" s="78" t="str">
-        <f>IF(AB$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>X</v>
       </c>
       <c r="AC32" s="77" t="str">
-        <f>IF(AC$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AD32" s="77" t="str">
-        <f>IF(AD$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AE32" s="77" t="str">
-        <f>IF(AE$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AF32" s="77" t="str">
-        <f>IF(AF$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AG32" s="32" t="str">
-        <f>IF(AG$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
       <c r="AH32" s="28" t="str">
-        <f>IF(AH$13="X","X","==")</f>
+        <f t="shared" si="8"/>
         <v>==</v>
       </c>
     </row>
     <row r="33" spans="1:34" s="2" customFormat="1">
       <c r="A33" s="27" t="str">
-        <f>IF(A$12="X","X","==")</f>
+        <f t="shared" ref="A33:AH33" si="9">IF(A$12="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B33" s="32" t="str">
-        <f>IF(B$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="C33" s="77" t="str">
-        <f>IF(C$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="D33" s="77" t="str">
-        <f>IF(D$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="E33" s="77" t="str">
-        <f>IF(E$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="F33" s="77" t="str">
-        <f>IF(F$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="G33" s="77" t="str">
-        <f>IF(G$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="H33" s="77" t="str">
-        <f>IF(H$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="I33" s="77" t="str">
-        <f>IF(I$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="J33" s="77" t="str">
-        <f>IF(J$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="K33" s="77" t="str">
-        <f>IF(K$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="L33" s="78" t="str">
-        <f>IF(L$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>X</v>
       </c>
       <c r="M33" s="77" t="str">
-        <f>IF(M$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="N33" s="77" t="str">
-        <f>IF(N$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="O33" s="77" t="str">
-        <f>IF(O$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="P33" s="77" t="str">
-        <f>IF(P$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="Q33" s="77" t="str">
-        <f>IF(Q$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="R33" s="77" t="str">
-        <f>IF(R$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="S33" s="77" t="str">
-        <f>IF(S$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="T33" s="77" t="str">
-        <f>IF(T$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="U33" s="77" t="str">
-        <f>IF(U$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="V33" s="77" t="str">
-        <f>IF(V$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="W33" s="77" t="str">
-        <f>IF(W$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="X33" s="77" t="str">
-        <f>IF(X$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="Y33" s="77" t="str">
-        <f>IF(Y$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="Z33" s="77" t="str">
-        <f>IF(Z$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AA33" s="77" t="str">
-        <f>IF(AA$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AB33" s="77" t="str">
-        <f>IF(AB$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AC33" s="77" t="str">
-        <f>IF(AC$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AD33" s="77" t="str">
-        <f>IF(AD$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AE33" s="77" t="str">
-        <f>IF(AE$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AF33" s="77" t="str">
-        <f>IF(AF$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AG33" s="32" t="str">
-        <f>IF(AG$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
       <c r="AH33" s="28" t="str">
-        <f>IF(AH$12="X","X","==")</f>
+        <f t="shared" si="9"/>
         <v>==</v>
       </c>
     </row>
     <row r="34" spans="1:34" s="2" customFormat="1">
       <c r="A34" s="27" t="str">
-        <f>IF(A$11="X","X","==")</f>
+        <f t="shared" ref="A34:AH34" si="10">IF(A$11="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B34" s="32" t="str">
-        <f>IF(B$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="C34" s="77" t="str">
-        <f>IF(C$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="D34" s="77" t="str">
-        <f>IF(D$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="E34" s="77" t="str">
-        <f>IF(E$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="F34" s="77" t="str">
-        <f>IF(F$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="G34" s="77" t="str">
-        <f>IF(G$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="H34" s="77" t="str">
-        <f>IF(H$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="I34" s="77" t="str">
-        <f>IF(I$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="J34" s="78" t="str">
-        <f>IF(J$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>X</v>
       </c>
       <c r="K34" s="77" t="str">
-        <f>IF(K$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="L34" s="77" t="str">
-        <f>IF(L$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="M34" s="77" t="str">
-        <f>IF(M$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="N34" s="78" t="str">
-        <f>IF(N$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>X</v>
       </c>
       <c r="O34" s="77" t="str">
-        <f>IF(O$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="P34" s="77" t="str">
-        <f>IF(P$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="Q34" s="77" t="str">
-        <f>IF(Q$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="R34" s="77" t="str">
-        <f>IF(R$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="S34" s="77" t="str">
-        <f>IF(S$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="T34" s="77" t="str">
-        <f>IF(T$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="U34" s="78" t="str">
-        <f>IF(U$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>X</v>
       </c>
       <c r="V34" s="77" t="str">
-        <f>IF(V$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="W34" s="77" t="str">
-        <f>IF(W$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="X34" s="77" t="str">
-        <f>IF(X$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="Y34" s="77" t="str">
-        <f>IF(Y$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="Z34" s="77" t="str">
-        <f>IF(Z$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AA34" s="77" t="str">
-        <f>IF(AA$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AB34" s="77" t="str">
-        <f>IF(AB$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AC34" s="77" t="str">
-        <f>IF(AC$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AD34" s="77" t="str">
-        <f>IF(AD$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AE34" s="77" t="str">
-        <f>IF(AE$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AF34" s="77" t="str">
-        <f>IF(AF$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AG34" s="32" t="str">
-        <f>IF(AG$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
       <c r="AH34" s="28" t="str">
-        <f>IF(AH$11="X","X","==")</f>
+        <f t="shared" si="10"/>
         <v>==</v>
       </c>
     </row>
     <row r="35" spans="1:34" s="2" customFormat="1">
       <c r="A35" s="27" t="str">
-        <f>IF(A$10="X","X","==")</f>
+        <f t="shared" ref="A35:AH35" si="11">IF(A$10="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B35" s="32" t="str">
-        <f>IF(B$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="C35" s="77" t="str">
-        <f>IF(C$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="D35" s="77" t="str">
-        <f>IF(D$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="E35" s="77" t="str">
-        <f>IF(E$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="F35" s="77" t="str">
-        <f>IF(F$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="G35" s="77" t="str">
-        <f>IF(G$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="H35" s="77" t="str">
-        <f>IF(H$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="I35" s="77" t="str">
-        <f>IF(I$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="J35" s="77" t="str">
-        <f>IF(J$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="K35" s="77" t="str">
-        <f>IF(K$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="L35" s="77" t="str">
-        <f>IF(L$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="M35" s="77" t="str">
-        <f>IF(M$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="N35" s="77" t="str">
-        <f>IF(N$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="O35" s="77" t="str">
-        <f>IF(O$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="P35" s="77" t="str">
-        <f>IF(P$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="Q35" s="77" t="str">
-        <f>IF(Q$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="R35" s="77" t="str">
-        <f>IF(R$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="S35" s="77" t="str">
-        <f>IF(S$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="T35" s="77" t="str">
-        <f>IF(T$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="U35" s="77" t="str">
-        <f>IF(U$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="V35" s="77" t="str">
-        <f>IF(V$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="W35" s="77" t="str">
-        <f>IF(W$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="X35" s="77" t="str">
-        <f>IF(X$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="Y35" s="77" t="str">
-        <f>IF(Y$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="Z35" s="77" t="str">
-        <f>IF(Z$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AA35" s="77" t="str">
-        <f>IF(AA$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AB35" s="77" t="str">
-        <f>IF(AB$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AC35" s="77" t="str">
-        <f>IF(AC$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AD35" s="77" t="str">
-        <f>IF(AD$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AE35" s="77" t="str">
-        <f>IF(AE$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AF35" s="77" t="str">
-        <f>IF(AF$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AG35" s="32" t="str">
-        <f>IF(AG$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
       <c r="AH35" s="28" t="str">
-        <f>IF(AH$10="X","X","==")</f>
+        <f t="shared" si="11"/>
         <v>==</v>
       </c>
     </row>
     <row r="36" spans="1:34" s="2" customFormat="1">
       <c r="A36" s="27" t="str">
-        <f>IF(A$9="X","X","==")</f>
+        <f t="shared" ref="A36:AH36" si="12">IF(A$9="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B36" s="32" t="str">
-        <f>IF(B$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="C36" s="77" t="str">
-        <f>IF(C$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="D36" s="77" t="str">
-        <f>IF(D$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="E36" s="77" t="str">
-        <f>IF(E$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="F36" s="77" t="str">
-        <f>IF(F$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="G36" s="77" t="str">
-        <f>IF(G$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="H36" s="77" t="str">
-        <f>IF(H$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="I36" s="77" t="str">
-        <f>IF(I$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="J36" s="77" t="str">
-        <f>IF(J$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="K36" s="77" t="str">
-        <f>IF(K$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="L36" s="77" t="str">
-        <f>IF(L$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="M36" s="77" t="str">
-        <f>IF(M$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="N36" s="78" t="str">
-        <f>IF(N$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>X</v>
       </c>
       <c r="O36" s="77" t="str">
-        <f>IF(O$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="P36" s="77" t="str">
-        <f>IF(P$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="Q36" s="77" t="str">
-        <f>IF(Q$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="R36" s="77" t="str">
-        <f>IF(R$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="S36" s="77" t="str">
-        <f>IF(S$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="T36" s="77" t="str">
-        <f>IF(T$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="U36" s="77" t="str">
-        <f>IF(U$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="V36" s="77" t="str">
-        <f>IF(V$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="W36" s="77" t="str">
-        <f>IF(W$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="X36" s="77" t="str">
-        <f>IF(X$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="Y36" s="77" t="str">
-        <f>IF(Y$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="Z36" s="77" t="str">
-        <f>IF(Z$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AA36" s="77" t="str">
-        <f>IF(AA$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AB36" s="77" t="str">
-        <f>IF(AB$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AC36" s="77" t="str">
-        <f>IF(AC$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AD36" s="77" t="str">
-        <f>IF(AD$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AE36" s="77" t="str">
-        <f>IF(AE$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AF36" s="77" t="str">
-        <f>IF(AF$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AG36" s="32" t="str">
-        <f>IF(AG$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
       <c r="AH36" s="28" t="str">
-        <f>IF(AH$9="X","X","==")</f>
+        <f t="shared" si="12"/>
         <v>==</v>
       </c>
     </row>
     <row r="37" spans="1:34" s="2" customFormat="1">
       <c r="A37" s="27" t="str">
-        <f>IF(A$8="X","X","==")</f>
+        <f t="shared" ref="A37:AH37" si="13">IF(A$8="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B37" s="32" t="str">
-        <f>IF(B$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="C37" s="77" t="str">
-        <f>IF(C$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="D37" s="77" t="str">
-        <f>IF(D$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="E37" s="77" t="str">
-        <f>IF(E$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="F37" s="77" t="str">
-        <f>IF(F$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="G37" s="77" t="str">
-        <f>IF(G$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="H37" s="77" t="str">
-        <f>IF(H$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="I37" s="77" t="str">
-        <f>IF(I$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="J37" s="77" t="str">
-        <f>IF(J$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="K37" s="77" t="str">
-        <f>IF(K$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="L37" s="77" t="str">
-        <f>IF(L$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="M37" s="77" t="str">
-        <f>IF(M$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="N37" s="78" t="str">
-        <f>IF(N$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>X</v>
       </c>
       <c r="O37" s="77" t="str">
-        <f>IF(O$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="P37" s="77" t="str">
-        <f>IF(P$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="Q37" s="77" t="str">
-        <f>IF(Q$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="R37" s="77" t="str">
-        <f>IF(R$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="S37" s="77" t="str">
-        <f>IF(S$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="T37" s="77" t="str">
-        <f>IF(T$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="U37" s="77" t="str">
-        <f>IF(U$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="V37" s="77" t="str">
-        <f>IF(V$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="W37" s="77" t="str">
-        <f>IF(W$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="X37" s="77" t="str">
-        <f>IF(X$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="Y37" s="77" t="str">
-        <f>IF(Y$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="Z37" s="77" t="str">
-        <f>IF(Z$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AA37" s="77" t="str">
-        <f>IF(AA$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AB37" s="77" t="str">
-        <f>IF(AB$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AC37" s="77" t="str">
-        <f>IF(AC$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AD37" s="77" t="str">
-        <f>IF(AD$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AE37" s="77" t="str">
-        <f>IF(AE$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AF37" s="77" t="str">
-        <f>IF(AF$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AG37" s="32" t="str">
-        <f>IF(AG$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
       <c r="AH37" s="28" t="str">
-        <f>IF(AH$8="X","X","==")</f>
+        <f t="shared" si="13"/>
         <v>==</v>
       </c>
     </row>
     <row r="38" spans="1:34" s="2" customFormat="1">
       <c r="A38" s="27" t="str">
-        <f>IF(A$7="X","X","==")</f>
+        <f t="shared" ref="A38:AH38" si="14">IF(A$7="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B38" s="32" t="str">
-        <f>IF(B$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="C38" s="77" t="str">
-        <f>IF(C$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="D38" s="77" t="str">
-        <f>IF(D$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="E38" s="78" t="str">
-        <f>IF(E$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>X</v>
       </c>
       <c r="F38" s="77" t="str">
-        <f>IF(F$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="G38" s="77" t="str">
-        <f>IF(G$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="H38" s="77" t="str">
-        <f>IF(H$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="I38" s="77" t="str">
-        <f>IF(I$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="J38" s="77" t="str">
-        <f>IF(J$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="K38" s="77" t="str">
-        <f>IF(K$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="L38" s="77" t="str">
-        <f>IF(L$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="M38" s="77" t="str">
-        <f>IF(M$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="N38" s="78" t="str">
-        <f>IF(N$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>X</v>
       </c>
       <c r="O38" s="77" t="str">
-        <f>IF(O$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="P38" s="77" t="str">
-        <f>IF(P$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="Q38" s="77" t="str">
-        <f>IF(Q$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="R38" s="77" t="str">
-        <f>IF(R$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="S38" s="77" t="str">
-        <f>IF(S$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="T38" s="77" t="str">
-        <f>IF(T$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="U38" s="77" t="str">
-        <f>IF(U$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="V38" s="77" t="str">
-        <f>IF(V$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="W38" s="77" t="str">
-        <f>IF(W$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="X38" s="77" t="str">
-        <f>IF(X$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="Y38" s="77" t="str">
-        <f>IF(Y$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="Z38" s="77" t="str">
-        <f>IF(Z$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AA38" s="77" t="str">
-        <f>IF(AA$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AB38" s="77" t="str">
-        <f>IF(AB$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AC38" s="77" t="str">
-        <f>IF(AC$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AD38" s="77" t="str">
-        <f>IF(AD$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AE38" s="77" t="str">
-        <f>IF(AE$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AF38" s="77" t="str">
-        <f>IF(AF$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AG38" s="32" t="str">
-        <f>IF(AG$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
       <c r="AH38" s="28" t="str">
-        <f>IF(AH$7="X","X","==")</f>
+        <f t="shared" si="14"/>
         <v>==</v>
       </c>
     </row>
     <row r="39" spans="1:34" s="2" customFormat="1">
       <c r="A39" s="27" t="str">
-        <f>IF(A$6="X","X","==")</f>
+        <f t="shared" ref="A39:AH39" si="15">IF(A$6="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B39" s="32" t="str">
-        <f>IF(B$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="C39" s="77" t="str">
-        <f>IF(C$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="D39" s="77" t="str">
-        <f>IF(D$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="E39" s="77" t="str">
-        <f>IF(E$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="F39" s="77" t="str">
-        <f>IF(F$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="G39" s="77" t="str">
-        <f>IF(G$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="H39" s="77" t="str">
-        <f>IF(H$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="I39" s="77" t="str">
-        <f>IF(I$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="J39" s="77" t="str">
-        <f>IF(J$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="K39" s="77" t="str">
-        <f>IF(K$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="L39" s="77" t="str">
-        <f>IF(L$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="M39" s="77" t="str">
-        <f>IF(M$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="N39" s="78" t="str">
-        <f>IF(N$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>X</v>
       </c>
       <c r="O39" s="77" t="str">
-        <f>IF(O$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="P39" s="77" t="str">
-        <f>IF(P$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="Q39" s="77" t="str">
-        <f>IF(Q$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="R39" s="77" t="str">
-        <f>IF(R$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="S39" s="77" t="str">
-        <f>IF(S$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="T39" s="77" t="str">
-        <f>IF(T$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="U39" s="77" t="str">
-        <f>IF(U$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="V39" s="77" t="str">
-        <f>IF(V$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="W39" s="77" t="str">
-        <f>IF(W$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="X39" s="77" t="str">
-        <f>IF(X$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="Y39" s="77" t="str">
-        <f>IF(Y$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="Z39" s="77" t="str">
-        <f>IF(Z$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AA39" s="77" t="str">
-        <f>IF(AA$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AB39" s="78" t="str">
-        <f>IF(AB$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>X</v>
       </c>
       <c r="AC39" s="77" t="str">
-        <f>IF(AC$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AD39" s="77" t="str">
-        <f>IF(AD$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AE39" s="77" t="str">
-        <f>IF(AE$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AF39" s="77" t="str">
-        <f>IF(AF$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AG39" s="32" t="str">
-        <f>IF(AG$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
       <c r="AH39" s="28" t="str">
-        <f>IF(AH$6="X","X","==")</f>
+        <f t="shared" si="15"/>
         <v>==</v>
       </c>
     </row>
     <row r="40" spans="1:34" s="2" customFormat="1">
       <c r="A40" s="27" t="str">
-        <f>IF(A$5="X","X","==")</f>
+        <f t="shared" ref="A40:AH40" si="16">IF(A$5="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B40" s="32" t="str">
-        <f>IF(B$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="C40" s="77" t="str">
-        <f>IF(C$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="D40" s="77" t="str">
-        <f>IF(D$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="E40" s="78" t="str">
-        <f>IF(E$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>X</v>
       </c>
       <c r="F40" s="77" t="str">
-        <f>IF(F$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="G40" s="77" t="str">
-        <f>IF(G$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="H40" s="77" t="str">
-        <f>IF(H$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="I40" s="77" t="str">
-        <f>IF(I$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="J40" s="78" t="str">
-        <f>IF(J$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>X</v>
       </c>
       <c r="K40" s="77" t="str">
-        <f>IF(K$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="L40" s="77" t="str">
-        <f>IF(L$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="M40" s="77" t="str">
-        <f>IF(M$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="N40" s="78" t="str">
-        <f>IF(N$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>X</v>
       </c>
       <c r="O40" s="77" t="str">
-        <f>IF(O$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="P40" s="77" t="str">
-        <f>IF(P$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="Q40" s="77" t="str">
-        <f>IF(Q$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="R40" s="77" t="str">
-        <f>IF(R$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="S40" s="77" t="str">
-        <f>IF(S$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="T40" s="77" t="str">
-        <f>IF(T$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="U40" s="77" t="str">
-        <f>IF(U$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="V40" s="77" t="str">
-        <f>IF(V$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="W40" s="77" t="str">
-        <f>IF(W$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="X40" s="77" t="str">
-        <f>IF(X$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="Y40" s="77" t="str">
-        <f>IF(Y$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="Z40" s="77" t="str">
-        <f>IF(Z$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AA40" s="77" t="str">
-        <f>IF(AA$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AB40" s="77" t="str">
-        <f>IF(AB$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AC40" s="77" t="str">
-        <f>IF(AC$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AD40" s="77" t="str">
-        <f>IF(AD$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AE40" s="78" t="str">
-        <f>IF(AE$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>X</v>
       </c>
       <c r="AF40" s="77" t="str">
-        <f>IF(AF$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AG40" s="32" t="str">
-        <f>IF(AG$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
       <c r="AH40" s="28" t="str">
-        <f>IF(AH$5="X","X","==")</f>
+        <f t="shared" si="16"/>
         <v>==</v>
       </c>
     </row>
     <row r="41" spans="1:34" s="2" customFormat="1">
       <c r="A41" s="27" t="str">
-        <f>IF(A$4="X","X","==")</f>
+        <f t="shared" ref="A41:AH41" si="17">IF(A$4="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B41" s="32" t="str">
-        <f>IF(B$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="C41" s="77" t="str">
-        <f>IF(C$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="D41" s="77" t="str">
-        <f>IF(D$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="E41" s="77" t="str">
-        <f>IF(E$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="F41" s="77" t="str">
-        <f>IF(F$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="G41" s="77" t="str">
-        <f>IF(G$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="H41" s="78" t="str">
-        <f>IF(H$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>X</v>
       </c>
       <c r="I41" s="77" t="str">
-        <f>IF(I$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="J41" s="77" t="str">
-        <f>IF(J$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="K41" s="77" t="str">
-        <f>IF(K$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="L41" s="77" t="str">
-        <f>IF(L$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="M41" s="77" t="str">
-        <f>IF(M$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="N41" s="78" t="str">
-        <f>IF(N$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>X</v>
       </c>
       <c r="O41" s="77" t="str">
-        <f>IF(O$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="P41" s="77" t="str">
-        <f>IF(P$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="Q41" s="77" t="str">
-        <f>IF(Q$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="R41" s="77" t="str">
-        <f>IF(R$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="S41" s="77" t="str">
-        <f>IF(S$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="T41" s="77" t="str">
-        <f>IF(T$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="U41" s="77" t="str">
-        <f>IF(U$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="V41" s="77" t="str">
-        <f>IF(V$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="W41" s="77" t="str">
-        <f>IF(W$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="X41" s="77" t="str">
-        <f>IF(X$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="Y41" s="77" t="str">
-        <f>IF(Y$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="Z41" s="77" t="str">
-        <f>IF(Z$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AA41" s="77" t="str">
-        <f>IF(AA$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AB41" s="77" t="str">
-        <f>IF(AB$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AC41" s="77" t="str">
-        <f>IF(AC$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AD41" s="77" t="str">
-        <f>IF(AD$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AE41" s="77" t="str">
-        <f>IF(AE$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AF41" s="77" t="str">
-        <f>IF(AF$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AG41" s="32" t="str">
-        <f>IF(AG$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
       <c r="AH41" s="28" t="str">
-        <f>IF(AH$4="X","X","==")</f>
+        <f t="shared" si="17"/>
         <v>==</v>
       </c>
     </row>
     <row r="42" spans="1:34" s="2" customFormat="1">
       <c r="A42" s="29" t="str">
-        <f>IF(A$3="X","X","==")</f>
+        <f t="shared" ref="A42:AH42" si="18">IF(A$3="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="B42" s="30" t="str">
-        <f>IF(B$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="C42" s="77" t="str">
-        <f>IF(C$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="D42" s="77" t="str">
-        <f>IF(D$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="E42" s="77" t="str">
-        <f>IF(E$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="F42" s="77" t="str">
-        <f>IF(F$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="G42" s="77" t="str">
-        <f>IF(G$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="H42" s="77" t="str">
-        <f>IF(H$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="I42" s="77" t="str">
-        <f>IF(I$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="J42" s="77" t="str">
-        <f>IF(J$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="K42" s="77" t="str">
-        <f>IF(K$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="L42" s="77" t="str">
-        <f>IF(L$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="M42" s="77" t="str">
-        <f>IF(M$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="N42" s="78" t="str">
-        <f>IF(N$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>X</v>
       </c>
       <c r="O42" s="77" t="str">
-        <f>IF(O$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="P42" s="77" t="str">
-        <f>IF(P$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="Q42" s="77" t="str">
-        <f>IF(Q$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="R42" s="77" t="str">
-        <f>IF(R$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="S42" s="77" t="str">
-        <f>IF(S$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="T42" s="77" t="str">
-        <f>IF(T$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="U42" s="77" t="str">
-        <f>IF(U$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="V42" s="77" t="str">
-        <f>IF(V$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="W42" s="77" t="str">
-        <f>IF(W$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="X42" s="77" t="str">
-        <f>IF(X$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="Y42" s="77" t="str">
-        <f>IF(Y$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="Z42" s="77" t="str">
-        <f>IF(Z$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AA42" s="77" t="str">
-        <f>IF(AA$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AB42" s="78" t="str">
-        <f>IF(AB$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>X</v>
       </c>
       <c r="AC42" s="77" t="str">
-        <f>IF(AC$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AD42" s="77" t="str">
-        <f>IF(AD$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AE42" s="77" t="str">
-        <f>IF(AE$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AF42" s="77" t="str">
-        <f>IF(AF$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AG42" s="30" t="str">
-        <f>IF(AG$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
       <c r="AH42" s="31" t="str">
-        <f>IF(AH$3="X","X","==")</f>
+        <f t="shared" si="18"/>
         <v>==</v>
       </c>
     </row>
@@ -5187,135 +5215,135 @@
         <v/>
       </c>
       <c r="B43" s="101" t="str">
-        <f t="shared" ref="B43:AH43" si="2">CONCATENATE(B$2)</f>
+        <f t="shared" ref="B43:AH43" si="19">CONCATENATE(B$2)</f>
         <v/>
       </c>
       <c r="C43" s="75" t="str">
-        <f>IF(C$2="X","X","==")</f>
+        <f t="shared" ref="C43:AF43" si="20">IF(C$2="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="D43" s="77" t="str">
-        <f>IF(D$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="E43" s="77" t="str">
-        <f>IF(E$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="F43" s="77" t="str">
-        <f>IF(F$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="G43" s="77" t="str">
-        <f>IF(G$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="H43" s="77" t="str">
-        <f>IF(H$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="I43" s="77" t="str">
-        <f>IF(I$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="J43" s="78" t="str">
-        <f>IF(J$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>X</v>
       </c>
       <c r="K43" s="77" t="str">
-        <f>IF(K$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="L43" s="77" t="str">
-        <f>IF(L$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="M43" s="77" t="str">
-        <f>IF(M$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="N43" s="78" t="str">
-        <f>IF(N$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>X</v>
       </c>
       <c r="O43" s="77" t="str">
-        <f>IF(O$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="P43" s="77" t="str">
-        <f>IF(P$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="Q43" s="77" t="str">
-        <f>IF(Q$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="R43" s="77" t="str">
-        <f>IF(R$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="S43" s="77" t="str">
-        <f>IF(S$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="T43" s="77" t="str">
-        <f>IF(T$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="U43" s="77" t="str">
-        <f>IF(U$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="V43" s="77" t="str">
-        <f>IF(V$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="W43" s="77" t="str">
-        <f>IF(W$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="X43" s="77" t="str">
-        <f>IF(X$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="Y43" s="77" t="str">
-        <f>IF(Y$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="Z43" s="77" t="str">
-        <f>IF(Z$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AA43" s="77" t="str">
-        <f>IF(AA$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AB43" s="77" t="str">
-        <f>IF(AB$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AC43" s="77" t="str">
-        <f>IF(AC$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AD43" s="77" t="str">
-        <f>IF(AD$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AE43" s="77" t="str">
-        <f>IF(AE$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AF43" s="76" t="str">
-        <f>IF(AF$2="X","X","==")</f>
+        <f t="shared" si="20"/>
         <v>==</v>
       </c>
       <c r="AG43" s="101" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AH43" s="104" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
@@ -5325,132 +5353,132 @@
         <v>A1</v>
       </c>
       <c r="B44" s="107" t="str">
-        <f t="shared" ref="B44:AH44" si="3">CONCATENATE(B$1)</f>
+        <f t="shared" ref="B44:AH44" si="21">CONCATENATE(B$1)</f>
         <v/>
       </c>
       <c r="C44" s="79" t="str">
-        <f>IF(C$1="X","X","==")</f>
+        <f t="shared" ref="C44:AF44" si="22">IF(C$1="X","X","==")</f>
         <v>==</v>
       </c>
       <c r="D44" s="80" t="str">
-        <f>IF(D$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="E44" s="80" t="str">
-        <f>IF(E$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="F44" s="80" t="str">
-        <f>IF(F$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="G44" s="80" t="str">
-        <f>IF(G$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="H44" s="80" t="str">
-        <f>IF(H$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="I44" s="80" t="str">
-        <f>IF(I$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="J44" s="80" t="str">
-        <f>IF(J$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="K44" s="80" t="str">
-        <f>IF(K$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="L44" s="80" t="str">
-        <f>IF(L$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="M44" s="80" t="str">
-        <f>IF(M$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="N44" s="81" t="str">
-        <f>IF(N$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>X</v>
       </c>
       <c r="O44" s="80" t="str">
-        <f>IF(O$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="P44" s="80" t="str">
-        <f>IF(P$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="Q44" s="80" t="str">
-        <f>IF(Q$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="R44" s="80" t="str">
-        <f>IF(R$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="S44" s="80" t="str">
-        <f>IF(S$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="T44" s="80" t="str">
-        <f>IF(T$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="U44" s="80" t="str">
-        <f>IF(U$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="V44" s="80" t="str">
-        <f>IF(V$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="W44" s="80" t="str">
-        <f>IF(W$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="X44" s="80" t="str">
-        <f>IF(X$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="Y44" s="80" t="str">
-        <f>IF(Y$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="Z44" s="80" t="str">
-        <f>IF(Z$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AA44" s="80" t="str">
-        <f>IF(AA$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AB44" s="80" t="str">
-        <f>IF(AB$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AC44" s="80" t="str">
-        <f>IF(AC$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AD44" s="80" t="str">
-        <f>IF(AD$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AE44" s="80" t="str">
-        <f>IF(AE$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AF44" s="82" t="str">
-        <f>IF(AF$1="X","X","==")</f>
+        <f t="shared" si="22"/>
         <v>==</v>
       </c>
       <c r="AG44" s="107"/>
       <c r="AH44" s="110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="21"/>
         <v>AH1</v>
       </c>
     </row>
@@ -5498,7 +5526,7 @@
   <dimension ref="A1:AH25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AR26" sqref="AR26"/>
+      <selection activeCell="AE2" sqref="AE2:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5578,7 +5606,9 @@
       <c r="AD2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="115"/>
+      <c r="AE2" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF2" s="56"/>
       <c r="AG2" s="113"/>
       <c r="AH2" s="116"/>
@@ -5618,7 +5648,9 @@
       <c r="AD3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="115"/>
+      <c r="AE3" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF3" s="114"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="7"/>
@@ -5660,7 +5692,9 @@
       <c r="AD4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="115"/>
+      <c r="AE4" s="67" t="s">
+        <v>1</v>
+      </c>
       <c r="AF4" s="114"/>
       <c r="AG4" s="39"/>
       <c r="AH4" s="9"/>
@@ -5946,7 +5980,9 @@
       <c r="AD11" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE11" s="115"/>
+      <c r="AE11" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF11" s="114"/>
       <c r="AG11" s="39"/>
       <c r="AH11" s="9"/>
@@ -5984,7 +6020,9 @@
       <c r="AD12" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE12" s="115"/>
+      <c r="AE12" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF12" s="114"/>
       <c r="AG12" s="39"/>
       <c r="AH12" s="9"/>
@@ -6022,8 +6060,8 @@
       <c r="AD13" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="AE13" s="115" t="s">
-        <v>12</v>
+      <c r="AE13" s="67" t="s">
+        <v>1</v>
       </c>
       <c r="AF13" s="114"/>
       <c r="AG13" s="39"/>
@@ -6299,7 +6337,7 @@
   <dimension ref="A1:AH30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+      <selection activeCell="AE2" sqref="AE2:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6390,7 +6428,9 @@
       <c r="AD2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="115"/>
+      <c r="AE2" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF2" s="56"/>
       <c r="AG2" s="113"/>
       <c r="AH2" s="124"/>
@@ -6434,7 +6474,9 @@
       <c r="AD3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="115"/>
+      <c r="AE3" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF3" s="114"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="125"/>
@@ -6484,7 +6526,9 @@
       <c r="AD4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="115"/>
+      <c r="AE4" s="67" t="s">
+        <v>1</v>
+      </c>
       <c r="AF4" s="114"/>
       <c r="AG4" s="39"/>
       <c r="AH4" s="126"/>
@@ -6886,7 +6930,9 @@
       <c r="AD11" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE11" s="115"/>
+      <c r="AE11" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF11" s="114"/>
       <c r="AG11" s="39"/>
       <c r="AH11" s="126"/>
@@ -6940,7 +6986,9 @@
       <c r="AD12" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE12" s="115"/>
+      <c r="AE12" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF12" s="114"/>
       <c r="AG12" s="39"/>
       <c r="AH12" s="126"/>
@@ -6992,8 +7040,8 @@
       <c r="AD13" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="AE13" s="115" t="s">
-        <v>12</v>
+      <c r="AE13" s="67" t="s">
+        <v>1</v>
       </c>
       <c r="AF13" s="114"/>
       <c r="AG13" s="39"/>
@@ -7339,7 +7387,7 @@
   <dimension ref="A1:AH35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AQ21" sqref="AQ21"/>
+      <selection activeCell="AZ9" sqref="AZ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7433,7 +7481,9 @@
       <c r="AD2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="114"/>
+      <c r="AE2" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF2" s="56"/>
       <c r="AG2" s="113"/>
       <c r="AH2" s="124"/>
@@ -7483,7 +7533,9 @@
       <c r="AD3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="114"/>
+      <c r="AE3" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF3" s="114"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="125"/>
@@ -7539,7 +7591,9 @@
       <c r="AD4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="114"/>
+      <c r="AE4" s="67" t="s">
+        <v>1</v>
+      </c>
       <c r="AF4" s="114"/>
       <c r="AG4" s="39"/>
       <c r="AH4" s="126"/>
@@ -7999,7 +8053,9 @@
       <c r="AD11" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE11" s="114"/>
+      <c r="AE11" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF11" s="114"/>
       <c r="AG11" s="39"/>
       <c r="AH11" s="126"/>
@@ -8057,7 +8113,9 @@
       <c r="AD12" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE12" s="114"/>
+      <c r="AE12" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF12" s="114"/>
       <c r="AG12" s="39"/>
       <c r="AH12" s="126"/>
@@ -8115,8 +8173,8 @@
       <c r="AD13" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="AE13" s="114" t="s">
-        <v>12</v>
+      <c r="AE13" s="67" t="s">
+        <v>1</v>
       </c>
       <c r="AF13" s="114"/>
       <c r="AG13" s="39"/>
@@ -8502,7 +8560,7 @@
   <dimension ref="A1:AH40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ4" sqref="AJ4"/>
+      <selection activeCell="BB18" sqref="BB18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8615,7 +8673,9 @@
       <c r="AD2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="114"/>
+      <c r="AE2" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF2" s="56"/>
       <c r="AG2" s="113"/>
       <c r="AH2" s="116"/>
@@ -8673,7 +8733,9 @@
       <c r="AD3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" s="114"/>
+      <c r="AE3" s="64" t="s">
+        <v>1</v>
+      </c>
       <c r="AF3" s="114"/>
       <c r="AG3" s="59"/>
       <c r="AH3" s="61"/>
@@ -8731,7 +8793,9 @@
       <c r="AD4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" s="114"/>
+      <c r="AE4" s="67" t="s">
+        <v>1</v>
+      </c>
       <c r="AF4" s="114"/>
       <c r="AG4" s="114"/>
       <c r="AH4" s="56"/>
@@ -9275,7 +9339,9 @@
       <c r="AD11" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE11" s="114"/>
+      <c r="AE11" s="63" t="s">
+        <v>1</v>
+      </c>
       <c r="AF11" s="114"/>
       <c r="AG11" s="55"/>
       <c r="AH11" s="56"/>
@@ -9347,8 +9413,8 @@
       <c r="AD12" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AE12" s="114" t="s">
-        <v>12</v>
+      <c r="AE12" s="64" t="s">
+        <v>1</v>
       </c>
       <c r="AF12" s="114"/>
       <c r="AG12" s="55"/>
@@ -9419,8 +9485,8 @@
       <c r="AD13" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="AE13" s="114" t="s">
-        <v>12</v>
+      <c r="AE13" s="67" t="s">
+        <v>1</v>
       </c>
       <c r="AF13" s="114"/>
       <c r="AG13" s="55"/>

</xml_diff>